<commit_message>
Update the 2024 EIS opt-out form
</commit_message>
<xml_diff>
--- a/GECO/EIS/2024-opt-out-form_annual.xlsx
+++ b/GECO/EIS/2024-opt-out-form_annual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwaldron\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B014DED2-5BBF-4871-B01A-9671F3366DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDDD20C-4953-48BE-B67E-3193C0A0A0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CACAC4CB-994E-45FD-A41B-F437926AC343}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CACAC4CB-994E-45FD-A41B-F437926AC343}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Guidelines</t>
   </si>
@@ -697,6 +697,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>*</t>
     </r>
@@ -705,6 +706,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Pb is not a threshold during annual EI years, but if a facility meets or exceeds the other thresholds during an annual EI year, a facility must report all pollutants including lead, if emitted, even during an annual year.</t>
     </r>
@@ -718,13 +720,16 @@
   </si>
   <si>
     <t>2024 Georgia Emission Inventory (EI) Opt-Out Form</t>
+  </si>
+  <si>
+    <t>Calculations attached.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,18 +806,15 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1270,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1353,14 +1355,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1680,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29ABFA58-0CCA-4D2D-9A1A-BAA0C97B9E12}">
   <dimension ref="B1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2566,7 +2561,7 @@
       <c r="L64" s="74"/>
       <c r="M64" s="75"/>
     </row>
-    <row r="65" customFormat="1" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="6">
@@ -2588,7 +2583,7 @@
   </sheetPr>
   <dimension ref="B1:N42"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17:G17"/>
     </sheetView>
   </sheetViews>
@@ -3079,7 +3074,7 @@
         <v>33</v>
       </c>
       <c r="G29" s="18" t="str" cm="1">
-        <f t="array" ref="G29">_xlfn.SWITCH(F29,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.")</f>
+        <f t="array" ref="G29">_xlfn.SWITCH(F29,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H29" s="32"/>
@@ -3109,7 +3104,7 @@
         <v>33</v>
       </c>
       <c r="G30" s="18" t="str" cm="1">
-        <f t="array" ref="G30">_xlfn.SWITCH(F30,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.")</f>
+        <f t="array" ref="G30">_xlfn.SWITCH(F30,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H30" s="33"/>
@@ -3139,7 +3134,7 @@
         <v>33</v>
       </c>
       <c r="G31" s="18" t="str" cm="1">
-        <f t="array" ref="G31">_xlfn.SWITCH(F31,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.")</f>
+        <f t="array" ref="G31">_xlfn.SWITCH(F31,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H31" s="18"/>
@@ -3151,7 +3146,9 @@
         <v>100</v>
       </c>
       <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
+      <c r="N31" s="24" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="39"/>
@@ -3167,7 +3164,7 @@
         <v>33</v>
       </c>
       <c r="G32" s="18" t="str" cm="1">
-        <f t="array" ref="G32">_xlfn.SWITCH(F32,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.")</f>
+        <f t="array" ref="G32">_xlfn.SWITCH(F32,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H32" s="18"/>
@@ -3227,7 +3224,7 @@
         <v>33</v>
       </c>
       <c r="G34" s="18" t="str" cm="1">
-        <f t="array" ref="G34">_xlfn.SWITCH(F34,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.")</f>
+        <f t="array" ref="G34">_xlfn.SWITCH(F34,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H34" s="33"/>
@@ -3256,8 +3253,8 @@
       <c r="F35" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="18" t="str">
-        <f t="shared" ref="G35:G36" si="1">IF(F35=$N$27,"Select PTE emissions justification",IF(F35=$N$28,"Provide permit # and permit condition limit.",IF(F35=$N$29,"Provide Title V application #.","No response required.")))</f>
+      <c r="G35" s="18" t="str" cm="1">
+        <f t="array" ref="G35">_xlfn.SWITCH(F35,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H35" s="32"/>
@@ -3286,8 +3283,8 @@
       <c r="F36" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="18" t="str">
-        <f t="shared" si="1"/>
+      <c r="G36" s="18" t="str" cm="1">
+        <f t="array" ref="G36">_xlfn.SWITCH(F36,"(Select)","Select PTE emissions justification",,"Select PTE emissions justification","Permit condition limit.","Provide permit # and permit condition limit.", "PTE from Title V application","Provide Title V application #.","Pollutant not emitted.","No response required.", "Calculations attached.", "Provide a basic sumary of the calcutional and attach calculations to Opt out report or include additional tab in form.")</f>
         <v>Select PTE emissions justification</v>
       </c>
       <c r="H36" s="18"/>
@@ -3358,7 +3355,7 @@
       <c r="G42" s="90"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mIUZw6Y0T9JRJH2WQCxFuNig7+/Xa1ojXN3Rh8imV5kvjuQINZM9GjxaRXt7wYYKzE6p/g29+PPJv92ihpZRzw==" saltValue="ocaNrh1zq+QyhnocvuHksA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6202sempOv53tUQfmfGRhwn6ZLSSDgAysCj40QJGggd0oZYm3GT0WqKlPQvXAW875CDxoaFZK70OFeE+arodvw==" saltValue="Lpeaiu2Ds77JPVOjJ175IQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="H33" name="Pb_triennial 2"/>
     <protectedRange sqref="E33:F33" name="Pb_triennial 1"/>
@@ -3388,10 +3385,7 @@
     <mergeCell ref="D37:E37"/>
   </mergeCells>
   <conditionalFormatting sqref="F33">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3400,7 +3394,7 @@
       <formula1>$K$16:$L$16</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29:F32 F34:F36" xr:uid="{A2D08CF8-C987-4C24-8A69-80E9FB248564}">
-      <formula1>$N$27:$N$30</formula1>
+      <formula1>$N$27:$N$31</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F33" xr:uid="{05B4E69A-B8F5-4D47-8FA2-B3779CE3DF01}">
       <formula1>$N$33:$N$36</formula1>
@@ -3412,6 +3406,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8f254427-4c97-4196-ad61-b055f5f542e4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6601c63a-c8bd-4021-b252-e7c1551181e0" xsi:nil="true"/>
+    <SharedWithUsers xmlns="6601c63a-c8bd-4021-b252-e7c1551181e0">
+      <UserInfo>
+        <DisplayName>Wang, Jing</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Phillips, Emily</DisplayName>
+        <AccountId>25</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Samad, Zarah</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Geonczy, Maria</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Gijon-felix, Ruben</DisplayName>
+        <AccountId>104</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5D33C20B60FB4094ACE0FF35E1F214" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99d3eb1ea416b4fb18268c3a8514a863">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f254427-4c97-4196-ad61-b055f5f542e4" xmlns:ns3="6601c63a-c8bd-4021-b252-e7c1551181e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="510609fad5ef17ac03e65ba9e8a9b4a4" ns2:_="" ns3:_="">
     <xsd:import namespace="8f254427-4c97-4196-ad61-b055f5f542e4"/>
@@ -3646,54 +3687,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8f254427-4c97-4196-ad61-b055f5f542e4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6601c63a-c8bd-4021-b252-e7c1551181e0" xsi:nil="true"/>
-    <SharedWithUsers xmlns="6601c63a-c8bd-4021-b252-e7c1551181e0">
-      <UserInfo>
-        <DisplayName>Wang, Jing</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Phillips, Emily</DisplayName>
-        <AccountId>25</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Samad, Zarah</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Geonczy, Maria</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Gijon-felix, Ruben</DisplayName>
-        <AccountId>104</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15691EED-C8CB-42C5-8703-DB06CB72D7AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6601c63a-c8bd-4021-b252-e7c1551181e0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8f254427-4c97-4196-ad61-b055f5f542e4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97718A8F-2529-4520-A1B0-F88A0D31D559}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED751CD-D225-43C5-A55E-2490E4ABAF5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3710,29 +3729,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15691EED-C8CB-42C5-8703-DB06CB72D7AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="6601c63a-c8bd-4021-b252-e7c1551181e0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8f254427-4c97-4196-ad61-b055f5f542e4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97718A8F-2529-4520-A1B0-F88A0D31D559}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>